<commit_message>
- Collected all info about Json on one page - Added description of Json Atom feeds - Added description of deleted entries in both Xml and JSON
git-svn-id: http://gforge.hl7.org/svn/fhir/trunk@569 2f0db536-2c49-4257-a3fa-e771ed206c19
</commit_message>
<xml_diff>
--- a/documents/projects/documents/CCDA resource mapping.xlsx
+++ b/documents/projects/documents/CCDA resource mapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="150" windowWidth="6390" windowHeight="8400"/>
+    <workbookView xWindow="480" yWindow="156" windowWidth="6396" windowHeight="8400" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Resources List" sheetId="7" r:id="rId1"/>
@@ -1237,22 +1237,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomRight" activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="7" t="s">
         <v>225</v>
       </c>
@@ -1260,7 +1260,7 @@
       <c r="C1" s="7"/>
       <c r="D1" s="7"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>237</v>
       </c>
@@ -1274,7 +1274,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>234</v>
       </c>
@@ -1288,7 +1288,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>234</v>
       </c>
@@ -1302,7 +1302,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>231</v>
       </c>
@@ -1316,7 +1316,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>231</v>
       </c>
@@ -1330,7 +1330,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>232</v>
       </c>
@@ -1344,7 +1344,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>232</v>
       </c>
@@ -1358,7 +1358,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>233</v>
       </c>
@@ -1372,7 +1372,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>201</v>
       </c>
@@ -1383,7 +1383,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>202</v>
       </c>
@@ -1397,7 +1397,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>105</v>
       </c>
@@ -1408,7 +1408,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>203</v>
       </c>
@@ -1419,7 +1419,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>203</v>
       </c>
@@ -1433,7 +1433,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>203</v>
       </c>
@@ -1447,7 +1447,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>203</v>
       </c>
@@ -1458,7 +1458,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>204</v>
       </c>
@@ -1472,7 +1472,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>204</v>
       </c>
@@ -1486,7 +1486,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>204</v>
       </c>
@@ -1500,7 +1500,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>204</v>
       </c>
@@ -1514,7 +1514,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>204</v>
       </c>
@@ -1528,9 +1528,9 @@
         <v>242</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B22" t="s">
         <v>208</v>
@@ -1539,7 +1539,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>204</v>
       </c>
@@ -1550,7 +1550,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>209</v>
       </c>
@@ -1561,7 +1561,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>205</v>
       </c>
@@ -1572,7 +1572,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>205</v>
       </c>
@@ -1583,7 +1583,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>205</v>
       </c>
@@ -1597,7 +1597,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>205</v>
       </c>
@@ -1608,7 +1608,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>210</v>
       </c>
@@ -1619,7 +1619,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>210</v>
       </c>
@@ -1630,7 +1630,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>206</v>
       </c>
@@ -1641,7 +1641,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>206</v>
       </c>
@@ -1655,7 +1655,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>206</v>
       </c>
@@ -1669,7 +1669,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>206</v>
       </c>
@@ -1680,7 +1680,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>206</v>
       </c>
@@ -1691,7 +1691,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>244</v>
       </c>
@@ -1724,21 +1724,21 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="40.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="1"/>
-    <col min="3" max="3" width="12.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="1"/>
-    <col min="5" max="5" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.88671875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.109375" style="1"/>
+    <col min="3" max="3" width="12.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.109375" style="1"/>
+    <col min="5" max="5" width="18.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="37" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
+    <col min="7" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>43</v>
       </c>
@@ -1758,7 +1758,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="144" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1778,7 +1778,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1798,7 +1798,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1815,7 +1815,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -1832,7 +1832,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>79</v>
       </c>
@@ -1846,7 +1846,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>93</v>
       </c>
@@ -1857,7 +1857,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>18</v>
       </c>
@@ -1874,7 +1874,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>104</v>
       </c>
@@ -1888,7 +1888,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
@@ -1905,7 +1905,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
@@ -1922,7 +1922,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
@@ -1939,7 +1939,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
@@ -1956,7 +1956,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>9</v>
       </c>
@@ -1973,7 +1973,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
@@ -1990,7 +1990,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>11</v>
       </c>
@@ -2010,7 +2010,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>171</v>
       </c>
@@ -2024,7 +2024,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>172</v>
       </c>
@@ -2038,7 +2038,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>12</v>
       </c>
@@ -2055,7 +2055,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="144" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>13</v>
       </c>
@@ -2075,7 +2075,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>14</v>
       </c>
@@ -2095,7 +2095,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>15</v>
       </c>
@@ -2112,7 +2112,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>134</v>
       </c>
@@ -2129,7 +2129,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>17</v>
       </c>
@@ -2149,7 +2149,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>137</v>
       </c>
@@ -2163,7 +2163,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>138</v>
       </c>
@@ -2177,7 +2177,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>19</v>
       </c>
@@ -2194,7 +2194,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>20</v>
       </c>
@@ -2211,7 +2211,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>163</v>
       </c>
@@ -2225,7 +2225,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>21</v>
       </c>
@@ -2242,7 +2242,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>23</v>
       </c>
@@ -2259,7 +2259,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>24</v>
       </c>
@@ -2279,7 +2279,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>25</v>
       </c>
@@ -2299,7 +2299,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>26</v>
       </c>
@@ -2316,7 +2316,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>155</v>
       </c>
@@ -2333,7 +2333,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>27</v>
       </c>
@@ -2350,7 +2350,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>28</v>
       </c>
@@ -2370,7 +2370,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>29</v>
       </c>
@@ -2387,7 +2387,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>30</v>
       </c>
@@ -2404,7 +2404,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>31</v>
       </c>
@@ -2421,7 +2421,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>32</v>
       </c>
@@ -2438,7 +2438,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>33</v>
       </c>
@@ -2455,7 +2455,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>34</v>
       </c>
@@ -2472,7 +2472,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>35</v>
       </c>
@@ -2492,7 +2492,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>36</v>
       </c>
@@ -2512,7 +2512,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>37</v>
       </c>
@@ -2532,7 +2532,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>38</v>
       </c>
@@ -2552,7 +2552,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>39</v>
       </c>
@@ -2572,7 +2572,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>40</v>
       </c>
@@ -2592,7 +2592,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>41</v>
       </c>
@@ -2612,7 +2612,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>42</v>
       </c>
@@ -2632,7 +2632,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>47</v>
       </c>
@@ -2649,7 +2649,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>135</v>
       </c>
@@ -2663,7 +2663,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>48</v>
       </c>
@@ -2683,7 +2683,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>49</v>
       </c>
@@ -2700,7 +2700,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>50</v>
       </c>
@@ -2717,7 +2717,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>51</v>
       </c>
@@ -2734,7 +2734,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>150</v>
       </c>
@@ -2748,7 +2748,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>182</v>
       </c>
@@ -2762,7 +2762,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>52</v>
       </c>
@@ -2779,7 +2779,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>53</v>
       </c>
@@ -2796,7 +2796,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>54</v>
       </c>
@@ -2813,7 +2813,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>55</v>
       </c>
@@ -2833,7 +2833,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>56</v>
       </c>
@@ -2850,7 +2850,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>57</v>
       </c>
@@ -2867,7 +2867,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>58</v>
       </c>
@@ -2884,7 +2884,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>59</v>
       </c>
@@ -2901,7 +2901,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>60</v>
       </c>
@@ -2918,7 +2918,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="69" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>61</v>
       </c>
@@ -2935,7 +2935,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="70" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>62</v>
       </c>
@@ -2952,7 +2952,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>63</v>
       </c>
@@ -2969,7 +2969,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>64</v>
       </c>
@@ -2986,7 +2986,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>65</v>
       </c>
@@ -3003,7 +3003,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>190</v>
       </c>
@@ -3017,7 +3017,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>191</v>
       </c>
@@ -3031,7 +3031,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>193</v>
       </c>
@@ -3045,7 +3045,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>194</v>
       </c>
@@ -3059,7 +3059,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>192</v>
       </c>
@@ -3073,7 +3073,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="79" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>66</v>
       </c>
@@ -3090,7 +3090,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>67</v>
       </c>
@@ -3107,7 +3107,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>68</v>
       </c>
@@ -3124,7 +3124,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>69</v>
       </c>
@@ -3156,14 +3156,14 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>86</v>
       </c>
@@ -3184,20 +3184,20 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="1"/>
-    <col min="7" max="7" width="10.28515625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="14.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.88671875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.109375" style="1"/>
+    <col min="7" max="7" width="10.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="10.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>83</v>
       </c>
@@ -3223,7 +3223,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>85</v>
       </c>
@@ -3249,7 +3249,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>87</v>
       </c>
@@ -3269,7 +3269,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>119</v>
       </c>
@@ -3292,7 +3292,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>174</v>
       </c>
@@ -3300,7 +3300,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>200</v>
       </c>
@@ -3320,7 +3320,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3334,15 +3334,15 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="14.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>83</v>
       </c>
@@ -3353,7 +3353,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>139</v>
       </c>
@@ -3364,7 +3364,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>140</v>
       </c>
@@ -3375,7 +3375,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>141</v>
       </c>
@@ -3395,38 +3395,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="1"/>
-    <col min="3" max="3" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="19.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.109375" style="1"/>
+    <col min="3" max="3" width="15.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" style="1" customWidth="1"/>
     <col min="6" max="6" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.140625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="11.85546875" style="1" customWidth="1"/>
-    <col min="14" max="14" width="9.140625" style="1"/>
-    <col min="15" max="15" width="11.85546875" style="1" customWidth="1"/>
-    <col min="16" max="17" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="22" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="16384" width="9.140625" style="1"/>
+    <col min="7" max="7" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="11.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="11.88671875" style="1" customWidth="1"/>
+    <col min="14" max="14" width="9.109375" style="1"/>
+    <col min="15" max="15" width="11.88671875" style="1" customWidth="1"/>
+    <col min="16" max="17" width="11.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="22" width="11.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>83</v>
       </c>
@@ -3500,7 +3500,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>85</v>
       </c>
@@ -3574,7 +3574,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>88</v>
       </c>
@@ -3648,7 +3648,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>94</v>
       </c>
@@ -3701,7 +3701,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>96</v>
       </c>
@@ -3712,7 +3712,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>98</v>
       </c>
@@ -3735,7 +3735,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>100</v>
       </c>
@@ -3755,7 +3755,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="8" spans="1:24" ht="90" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>101</v>
       </c>
@@ -3775,7 +3775,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>102</v>
       </c>
@@ -3795,7 +3795,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>87</v>
       </c>
@@ -3836,7 +3836,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>106</v>
       </c>
@@ -3847,7 +3847,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="12" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>108</v>
       </c>
@@ -3864,7 +3864,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="13" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>109</v>
       </c>
@@ -3878,7 +3878,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>115</v>
       </c>
@@ -3895,7 +3895,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="15" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>116</v>
       </c>
@@ -3915,7 +3915,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="16" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>117</v>
       </c>
@@ -3929,7 +3929,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>121</v>
       </c>
@@ -3940,7 +3940,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>125</v>
       </c>
@@ -3951,7 +3951,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>145</v>
       </c>
@@ -3959,7 +3959,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>146</v>
       </c>
@@ -3967,7 +3967,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>166</v>
       </c>
@@ -3978,7 +3978,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>179</v>
       </c>

</xml_diff>